<commit_message>
new sample file added for goods and sample
</commit_message>
<xml_diff>
--- a/public/productGoodsSample.xlsx
+++ b/public/productGoodsSample.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27628"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Project\hues-frontend\public\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFDAD5B-EC43-4AA8-9F6C-34D5AF06F6E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Sr. No</t>
   </si>
@@ -56,13 +51,25 @@
   </si>
   <si>
     <t>IGST (%)</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Length</t>
+  </si>
+  <si>
+    <t>Breadth</t>
+  </si>
+  <si>
+    <t>Height</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -72,6 +79,11 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -93,29 +105,130 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
+      <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
+      <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center"/>
+      <protection/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
+      <protection/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -423,29 +536,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7044A5AE-1D53-4D1A-AB21-1C061CDEDF88}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7044a5ae-1d53-4d1a-ab21-1c061cdedf88}">
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="25.109375" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="14.7142857142857" customWidth="1"/>
+    <col min="4" max="4" width="25.1428571428571" customWidth="1"/>
+    <col min="5" max="5" width="21.2857142857143" customWidth="1"/>
     <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.2857142857143" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" customWidth="1"/>
-    <col min="11" max="11" width="11.109375" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" customWidth="1"/>
+    <col min="10" max="10" width="12.5714285714286" customWidth="1"/>
+    <col min="11" max="11" width="11.1428571428571" customWidth="1"/>
+    <col min="12" max="12" width="9.71428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="12.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -476,22 +589,33 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4"/>
+      <c r="M1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:10" ht="12.75" customHeight="1">
+      <c r="A2" s="4"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="J2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>